<commit_message>
57 - credit applications
</commit_message>
<xml_diff>
--- a/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
+++ b/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B61C93A-34B8-1E44-ABCD-B3A5517805EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A6D8A-E677-FA4A-B87F-A05D13ED0E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{515AB8EB-AA8F-2C43-9A6B-8AF89862BE7B}"/>
+    <workbookView xWindow="5620" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{515AB8EB-AA8F-2C43-9A6B-8AF89862BE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
-  <si>
-    <t>instructions go here</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Make</t>
   </si>
@@ -56,15 +53,45 @@
   </si>
   <si>
     <t>Model Year</t>
+  </si>
+  <si>
+    <t>Please fill out the "ZEVs Supplied" sheet.</t>
+  </si>
+  <si>
+    <t>With respect to the "ZEVs Supplied" sheet:</t>
+  </si>
+  <si>
+    <t>(1) Only the vehicles listed in the "Valid Vehicles" sheet may be used.</t>
+  </si>
+  <si>
+    <t>(2) VINs must be exactly 17 characters.</t>
+  </si>
+  <si>
+    <t>(4) No more than 2000 records may be entered.</t>
+  </si>
+  <si>
+    <t>(3) Dates must be of the YYYY-MM-DD format.</t>
+  </si>
+  <si>
+    <t>With respect to this entire document:</t>
+  </si>
+  <si>
+    <t>(1) Please do not change the existing cell formatting.</t>
+  </si>
+  <si>
+    <t>(2) Please do not add any cell formatting.</t>
+  </si>
+  <si>
+    <t>(3) Please do not add any data validation.</t>
+  </si>
+  <si>
+    <t>(4) Please do not change any of the sheet names or header names.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,7 +131,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,18 +466,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC198ED0-26FB-CD41-B8E5-195ADA9EB37D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -474,13 +551,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -506,28 +583,22 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E2001" xr:uid="{4F0E0A76-19D3-D74F-8A2A-EA71E6C9EC23}">
-      <formula1>39814</formula1>
-      <formula2>52963</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2520 and 138 - table refinements/highlighting
</commit_message>
<xml_diff>
--- a/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
+++ b/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/repos/zeva2/next/app/credit-application/lib/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A6D8A-E677-FA4A-B87F-A05D13ED0E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432FF07-EC17-4644-B23C-0B0129A47B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{515AB8EB-AA8F-2C43-9A6B-8AF89862BE7B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Make</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>(4) Please do not change any of the sheet names or header names.</t>
+  </si>
+  <si>
+    <t>(4) Dates must be on or after January 2nd, 2018.</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC198ED0-26FB-CD41-B8E5-195ADA9EB37D}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -527,6 +530,11 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2520 and 138 - table refinements/highlighting (#169)
* 2520 and 138 - table refinements/highlighting

* formatting
</commit_message>
<xml_diff>
--- a/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
+++ b/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/repos/zeva2/next/app/credit-application/lib/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A6D8A-E677-FA4A-B87F-A05D13ED0E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432FF07-EC17-4644-B23C-0B0129A47B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{515AB8EB-AA8F-2C43-9A6B-8AF89862BE7B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Make</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>(4) Please do not change any of the sheet names or header names.</t>
+  </si>
+  <si>
+    <t>(4) Dates must be on or after January 2nd, 2018.</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC198ED0-26FB-CD41-B8E5-195ADA9EB37D}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -527,6 +530,11 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
175: attachment changes + some refactoring (#273)
* initial commit

* second commit

* third commit

* fourth commit

* fifth commit

* sixth commit
</commit_message>
<xml_diff>
--- a/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
+++ b/next/app/credit-application/lib/templates/credit_application_supplier_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/zeva/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F76712B-D2DB-4849-80CB-FF4DA369D9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8076AD1-C586-A140-8654-293609F10DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="2760" windowWidth="27240" windowHeight="16440" xr2:uid="{515AB8EB-AA8F-2C43-9A6B-8AF89862BE7B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Make</t>
   </si>
@@ -61,18 +61,6 @@
     <t>With respect to the "ZEVs Supplied" sheet:</t>
   </si>
   <si>
-    <t>(1) Only the vehicles listed in the "Valid Vehicles" sheet may be used.</t>
-  </si>
-  <si>
-    <t>(2) VINs must be exactly 17 characters.</t>
-  </si>
-  <si>
-    <t>(4) No more than 2000 records may be entered.</t>
-  </si>
-  <si>
-    <t>(3) Dates must be of the YYYY-MM-DD format.</t>
-  </si>
-  <si>
     <t>With respect to this entire document:</t>
   </si>
   <si>
@@ -86,6 +74,21 @@
   </si>
   <si>
     <t>(4) Please do not change any of the sheet names or header names.</t>
+  </si>
+  <si>
+    <t>(2) Only the vehicles listed in the "Valid Vehicles" sheet may be used.</t>
+  </si>
+  <si>
+    <t>(3) VINs must be exactly 17 characters.</t>
+  </si>
+  <si>
+    <t>(4) Dates must be of the YYYY-MM-DD format.</t>
+  </si>
+  <si>
+    <t>(5) No more than 2000 records may be entered.</t>
+  </si>
+  <si>
+    <t>(1) If a row is not empty, then no cell within that row may be empty.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC198ED0-26FB-CD41-B8E5-195ADA9EB37D}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,27 +488,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -515,22 +518,27 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3112B8CE-1A89-1B4B-9407-70E951BEE2A0}">
   <dimension ref="A1:E2001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>